<commit_message>
update all experiment data
</commit_message>
<xml_diff>
--- a/recording/cifar10_4_subnetworks.xlsx
+++ b/recording/cifar10_4_subnetworks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator.USER-20190214OB\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wsl_in_win\Tensor_Layer_Neural_Networks\release\recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8726CC8-7C04-4808-9FB1-F34B0AC56D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AA11C9-58F3-45B3-AEB5-038CDED03680}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectral_conv_tensor_9L_subnets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Test Acc:</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>subnet3</t>
-  </si>
-  <si>
-    <t>subnet4</t>
   </si>
   <si>
     <t>Test Loss:</t>
@@ -60,11 +57,23 @@
   <si>
     <t>Fusing Train Loss:</t>
   </si>
+  <si>
+    <t>subnet0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>subnet1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>subnet2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1012,10 +1021,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2400" workbookViewId="0">
+      <selection activeCell="O2425" sqref="O2425"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1024,16 +1035,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6138,19 +6149,19 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B302" t="s">
+        <v>12</v>
+      </c>
+      <c r="C302" t="s">
         <v>1</v>
       </c>
-      <c r="C302" t="s">
+      <c r="D302" t="s">
         <v>2</v>
       </c>
-      <c r="D302" t="s">
+      <c r="E302" t="s">
         <v>3</v>
-      </c>
-      <c r="E302" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
@@ -11255,10 +11266,10 @@
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
+        <v>5</v>
+      </c>
+      <c r="B603" t="s">
         <v>6</v>
-      </c>
-      <c r="B603" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.2">
@@ -13663,10 +13674,10 @@
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B904" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
@@ -16071,19 +16082,19 @@
     </row>
     <row r="1205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1205" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1205" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1205" t="s">
         <v>1</v>
       </c>
-      <c r="C1205" t="s">
+      <c r="D1205" t="s">
         <v>2</v>
       </c>
-      <c r="D1205" t="s">
+      <c r="E1205" t="s">
         <v>3</v>
-      </c>
-      <c r="E1205" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="1206" spans="1:5" x14ac:dyDescent="0.2">
@@ -21188,19 +21199,19 @@
     </row>
     <row r="1506" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1506" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1506" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1506" t="s">
         <v>1</v>
       </c>
-      <c r="C1506" t="s">
+      <c r="D1506" t="s">
         <v>2</v>
       </c>
-      <c r="D1506" t="s">
+      <c r="E1506" t="s">
         <v>3</v>
-      </c>
-      <c r="E1506" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="1507" spans="1:5" x14ac:dyDescent="0.2">
@@ -26305,7 +26316,7 @@
     </row>
     <row r="1807" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1807" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1808" spans="1:5" x14ac:dyDescent="0.2">
@@ -28710,7 +28721,7 @@
     </row>
     <row r="2108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2108" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2109" spans="1:2" x14ac:dyDescent="0.2">
@@ -31116,5 +31127,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>